<commit_message>
Updated 'ValidLogin' test case with Data Drive using Excel
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCase1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
   <si>
-    <t>Gururaj</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,14 +377,20 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 'InvalidLogin' Test Case with Data Driven Added sheet 'InvalidLogin' in the input.xlsx Workbook
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>UserName</t>
   </si>
@@ -368,8 +368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,12 +400,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>